<commit_message>
add cdate time and name columns
</commit_message>
<xml_diff>
--- a/outputs/output.xlsx
+++ b/outputs/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,16 @@
           <t>Language</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Followup / Modify Date/Time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,292 +466,14 @@
           <t>English</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>English</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Hindi</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Hindi</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-04-21 10:47:00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Pravin Pawar</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add description column and style wb
</commit_message>
<xml_diff>
--- a/outputs/output.xlsx
+++ b/outputs/output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -55,10 +55,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,13 +434,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="80" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -439,51 +456,75 @@
           <t>Actions</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Language</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Followup / Modify Date/Time</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Lead Quality</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Add Pipeline, Potential IP Lead, call, Share Lead, Lead Details, Official Chat, Send Pay Fee Link, Send Mailer, Training Docs, Create Demo Request</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>English</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>2024-04-21 10:47:00</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>Pravin Pawar</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>Paid</t>
+        </is>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">29/06/2024 11:09am - 14000 paid , 6000 pending
+29/06/2024 09:52am - 1600 pay
+24/06/2024 05:03pm - register with 1000, pending 19000
+24/06/2024 05:03pm - register with 1000
+13/06/2024 02:39pm - npu
+01/06/2024 02:32pm - call at 6 pm today
+21/05/2024 06:14pm - npu
+09/05/2024 05:36pm - npu
+09/05/2024 04:32pm - call at 5:30
+28/04/2024 06:26pm - npu
+28/04/2024 06:26pm - npu
+16/04/2024 11:27am - npu , call again
+13/04/2024 10:52am - 10 yrs exp. in pp call again on 21 april
+13/04/2024 10:47am - reference of omkar. had a discusion , he will enroll in month end of april.
+</t>
         </is>
       </c>
     </row>

</xml_diff>